<commit_message>
Modificacion para el dashboard
</commit_message>
<xml_diff>
--- a/datos/setup/parametros.xlsx
+++ b/datos/setup/parametros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared\P\Cuervo\shiny\datos\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0060572-36EF-47A7-8C38-A430AFA1B813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA85C3AA-6301-40D3-9EDA-ABAEDB537445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>domestico_fechas</t>
   </si>
@@ -150,12 +150,6 @@
     <t>zsdr141</t>
   </si>
   <si>
-    <t>Oficina de Ventas..4</t>
-  </si>
-  <si>
-    <t>Cliente Destinatario..30</t>
-  </si>
-  <si>
     <t>Nombre Región</t>
   </si>
   <si>
@@ -207,7 +201,22 @@
     <t>usa_aux_y</t>
   </si>
   <si>
-    <t>Pedido SAP::Material</t>
+    <t>Pedido::Material</t>
+  </si>
+  <si>
+    <t>Ctd. Ped.</t>
+  </si>
+  <si>
+    <t>Cajas Naturales</t>
+  </si>
+  <si>
+    <t>Pedido SAP::Código SAP</t>
+  </si>
+  <si>
+    <t>Cliente Destinatario...30</t>
+  </si>
+  <si>
+    <t>Oficina de Ventas...4</t>
   </si>
 </sst>
 </file>
@@ -688,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,13 +791,13 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" t="s">
         <v>57</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>59</v>
       </c>
       <c r="AC1" t="s">
         <v>25</v>
@@ -859,51 +868,51 @@
         <v>40</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="W2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="AA2" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="AD2" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -913,35 +922,37 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="N3" s="6"/>
       <c r="O3" s="1"/>
       <c r="P3" s="6"/>
       <c r="T3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" t="s">
         <v>50</v>
-      </c>
-      <c r="V3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -954,13 +965,15 @@
         <v>38</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="T4" s="1"/>
       <c r="X4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="30" x14ac:dyDescent="0.25">
@@ -968,10 +981,10 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>

</xml_diff>

<commit_message>
Cambios para funcionamiento de benchmark
</commit_message>
<xml_diff>
--- a/datos/setup/parametros.xlsx
+++ b/datos/setup/parametros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared\P\Cuervo\shiny\datos\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA85C3AA-6301-40D3-9EDA-ABAEDB537445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998605A-543D-4B19-951B-E508CCED0AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,8 +846,8 @@
       <c r="L2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>37</v>
+      <c r="M2" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>37</v>
@@ -856,7 +856,7 @@
         <v>38</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
         <v>39</v>
@@ -925,8 +925,8 @@
         <v>47</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>59</v>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="1"/>
@@ -995,7 +995,6 @@
       <c r="J5" s="7"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>

</xml_diff>